<commit_message>
Updated bug in excels
</commit_message>
<xml_diff>
--- a/excels/Bath.xlsx
+++ b/excels/Bath.xlsx
@@ -2646,7 +2646,7 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>2811.608108215167</v>
@@ -2675,7 +2675,7 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="1">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>2745.825323059388</v>
@@ -2704,7 +2704,7 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="1">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>2745.825323059388</v>
@@ -2733,7 +2733,7 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="1">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>2745.825323059388</v>
@@ -2762,7 +2762,7 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="1">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>3714.938449418363</v>
@@ -2791,7 +2791,7 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="1">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>3648.424582279681</v>
@@ -2820,7 +2820,7 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="1">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>3648.424582279681</v>
@@ -2849,7 +2849,7 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="1">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>3648.424582279681</v>
@@ -2878,7 +2878,7 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="1">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>3648.424582279681</v>
@@ -2907,7 +2907,7 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="1">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>3648.424582279681</v>
@@ -2936,7 +2936,7 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="1">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>3648.424582279681</v>
@@ -2965,7 +2965,7 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="1">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>3648.424582279681</v>
@@ -2994,7 +2994,7 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="1">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>2452.647113553671</v>
@@ -3023,7 +3023,7 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="1">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>4946.702716802681</v>
@@ -3052,7 +3052,7 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="1">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>4946.702716802681</v>
@@ -3081,7 +3081,7 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="1">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>4946.702716802681</v>
@@ -3110,7 +3110,7 @@
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="1">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>4946.702716802681</v>
@@ -3139,7 +3139,7 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="1">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>4946.702716802681</v>
@@ -3168,7 +3168,7 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="1">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="B21">
         <v>4946.702716802681</v>
@@ -3197,7 +3197,7 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="1">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="B22">
         <v>2466.619125095669</v>
@@ -3226,7 +3226,7 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="1">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="B23">
         <v>7781.45471603958</v>
@@ -3255,7 +3255,7 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="1">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B24">
         <v>7781.45471603958</v>
@@ -3284,7 +3284,7 @@
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="1">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="B25">
         <v>7781.45471603958</v>
@@ -3313,7 +3313,7 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="1">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="B26">
         <v>7781.45471603958</v>
@@ -3342,7 +3342,7 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="1">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="B27">
         <v>2524.623287671233</v>
@@ -3371,7 +3371,7 @@
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="1">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="B28">
         <v>7781.45471603958</v>
@@ -3400,7 +3400,7 @@
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="1">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="B29">
         <v>11468.55147929114</v>
@@ -3429,7 +3429,7 @@
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="1">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="B30">
         <v>3781.136294410754</v>
@@ -3458,7 +3458,7 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="1">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="B31">
         <v>3781.136294410754</v>
@@ -3487,7 +3487,7 @@
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="1">
-        <v>58</v>
+        <v>30</v>
       </c>
       <c r="B32">
         <v>12535.41941084526</v>
@@ -3516,7 +3516,7 @@
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="1">
-        <v>59</v>
+        <v>31</v>
       </c>
       <c r="B33">
         <v>12535.41941084526</v>
@@ -3545,7 +3545,7 @@
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="1">
-        <v>62</v>
+        <v>32</v>
       </c>
       <c r="B34">
         <v>12535.41941084526</v>
@@ -3574,7 +3574,7 @@
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="1">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="B35">
         <v>3535.006395297748</v>
@@ -3603,7 +3603,7 @@
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="1">
-        <v>66</v>
+        <v>34</v>
       </c>
       <c r="B36">
         <v>3385.801072066707</v>
@@ -3632,7 +3632,7 @@
     </row>
     <row r="37" spans="1:9">
       <c r="A37" s="1">
-        <v>69</v>
+        <v>35</v>
       </c>
       <c r="B37">
         <v>3491.230094025523</v>
@@ -3661,7 +3661,7 @@
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="1">
-        <v>70</v>
+        <v>36</v>
       </c>
       <c r="B38">
         <v>3535.006395297748</v>
@@ -3690,7 +3690,7 @@
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="1">
-        <v>71</v>
+        <v>37</v>
       </c>
       <c r="B39">
         <v>5475.139671350043</v>
@@ -3719,7 +3719,7 @@
     </row>
     <row r="40" spans="1:9">
       <c r="A40" s="1">
-        <v>74</v>
+        <v>38</v>
       </c>
       <c r="B40">
         <v>3095.699821322216</v>
@@ -3748,7 +3748,7 @@
     </row>
     <row r="41" spans="1:9">
       <c r="A41" s="1">
-        <v>75</v>
+        <v>39</v>
       </c>
       <c r="B41">
         <v>3997.879690291841</v>
@@ -3777,7 +3777,7 @@
     </row>
     <row r="42" spans="1:9">
       <c r="A42" s="1">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="B42">
         <v>3997.879690291841</v>
@@ -3806,7 +3806,7 @@
     </row>
     <row r="43" spans="1:9">
       <c r="A43" s="1">
-        <v>77</v>
+        <v>41</v>
       </c>
       <c r="B43">
         <v>3189.255509231686</v>
@@ -3835,7 +3835,7 @@
     </row>
     <row r="44" spans="1:9">
       <c r="A44" s="1">
-        <v>78</v>
+        <v>42</v>
       </c>
       <c r="B44">
         <v>3997.879690291841</v>
@@ -3864,7 +3864,7 @@
     </row>
     <row r="45" spans="1:9">
       <c r="A45" s="1">
-        <v>79</v>
+        <v>43</v>
       </c>
       <c r="B45">
         <v>3997.879690291841</v>
@@ -3893,7 +3893,7 @@
     </row>
     <row r="46" spans="1:9">
       <c r="A46" s="1">
-        <v>80</v>
+        <v>44</v>
       </c>
       <c r="B46">
         <v>3997.879690291841</v>
@@ -3922,7 +3922,7 @@
     </row>
     <row r="47" spans="1:9">
       <c r="A47" s="1">
-        <v>81</v>
+        <v>45</v>
       </c>
       <c r="B47">
         <v>3095.699821322216</v>
@@ -3951,7 +3951,7 @@
     </row>
     <row r="48" spans="1:9">
       <c r="A48" s="1">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="B48">
         <v>3997.879690291841</v>
@@ -3980,7 +3980,7 @@
     </row>
     <row r="49" spans="1:9">
       <c r="A49" s="1">
-        <v>83</v>
+        <v>47</v>
       </c>
       <c r="B49">
         <v>3997.879690291841</v>

</xml_diff>